<commit_message>
Revert "agregado de alianz"
This reverts commit 591da73508f1907f4c096310ed5678fc2f4b3679.
</commit_message>
<xml_diff>
--- a/Libro2.xlsx
+++ b/Libro2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Prueba basica de excel en git</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Zurich</t>
-  </si>
-  <si>
-    <t>allianz</t>
   </si>
 </sst>
 </file>
@@ -382,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,17 +439,6 @@
       </c>
       <c r="C8" s="1">
         <v>42464</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>61</v>
-      </c>
-      <c r="C9" s="1">
-        <v>42465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "agregado de alianz""
This reverts commit 73bae94b5a4a60f181e5500bc4f31c6a609b3d27.
</commit_message>
<xml_diff>
--- a/Libro2.xlsx
+++ b/Libro2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Prueba basica de excel en git</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Zurich</t>
+  </si>
+  <si>
+    <t>allianz</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +442,17 @@
       </c>
       <c r="C8" s="1">
         <v>42464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>61</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>